<commit_message>
Package for use in browser
</commit_message>
<xml_diff>
--- a/test/out/example.xlsx
+++ b/test/out/example.xlsx
@@ -15,24 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>I am title</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -373,163 +356,68 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1">
         <v>1</v>
       </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
       <c r="C1" t="s">
+        <v>-1</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1"/>
-      <c r="F1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
-      <c r="J1"/>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2"/>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>4</v>
       </c>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
+      <c r="C3">
+        <v>NaN</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>